<commit_message>
Commit 1.1 Add Test Categories
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataExcel.xlsx
+++ b/src/test/resources/testdata/DataExcel.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_New\CRM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796E734E-69B0-4C93-8241-B1B774AF1614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6CCD5-5125-4B22-A910-08DBD996EA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Add_New_Prod" sheetId="3" r:id="rId2"/>
     <sheet name="List_Prods" sheetId="5" r:id="rId3"/>
     <sheet name="Edit_Created_Prod" sheetId="6" r:id="rId4"/>
+    <sheet name="Create_Category" sheetId="7" r:id="rId5"/>
+    <sheet name="List_Category" sheetId="9" r:id="rId6"/>
+    <sheet name="Edit_Created_Category" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
   <si>
     <t>TESTCASEID</t>
   </si>
@@ -298,18 +301,142 @@
   </si>
   <si>
     <t>editProdFailureWithNotEmptyData</t>
+  </si>
+  <si>
+    <t>CATEGORY_NAME</t>
+  </si>
+  <si>
+    <t>PARENT_CATEGORY</t>
+  </si>
+  <si>
+    <t>ORDER_NUMBER</t>
+  </si>
+  <si>
+    <t>CATEGORY_TITLE</t>
+  </si>
+  <si>
+    <t>CATEGORY_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>FILTERING_ATTRIBUTE</t>
+  </si>
+  <si>
+    <t>addCategorySuccessfullyWithAllField</t>
+  </si>
+  <si>
+    <t>addCategorySuccessfullyWithRequiredField</t>
+  </si>
+  <si>
+    <t>addCategoryFailureWithNotRequiredField</t>
+  </si>
+  <si>
+    <t>addCategoryFailureWithEmptyField</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>LINK_LIST_CATEGORY</t>
+  </si>
+  <si>
+    <t>LINK_CREATE_CATEGORY</t>
+  </si>
+  <si>
+    <t>https://demo.activeitzone.com/ecommerce/admin/categories/create</t>
+  </si>
+  <si>
+    <t>https://demo.activeitzone.com/ecommerce/admin/categories</t>
+  </si>
+  <si>
+    <t>Xiaomi Global Home</t>
+  </si>
+  <si>
+    <t>Every precious moment in life deserves the best shot -whether it's in motion or still, bright or dark.We are ready to make moments mega, and so should you.</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>LG pans</t>
+  </si>
+  <si>
+    <t>https://demo.activeitzone.com/ecommerce/admin/categories/edit</t>
+  </si>
+  <si>
+    <t>LINK_EDIT_CATEGORY</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>Coolmate</t>
+  </si>
+  <si>
+    <t>Coolmate care and share</t>
+  </si>
+  <si>
+    <t>We believe no one should go hungry.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -425,27 +552,27 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -453,6 +580,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -899,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6C99E-9CF1-4595-AA6D-733C4803C7D5}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W12" sqref="W12:W14"/>
     </sheetView>
   </sheetViews>
@@ -1194,7 +1336,7 @@
       <c r="A6" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{B929C893-4433-4C03-B26F-B5559008C652}"/>
     <hyperlink ref="E4" r:id="rId2" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{403B3D36-2600-46C5-A541-4D32894C29EF}"/>
@@ -1704,4 +1846,820 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DFD8CB-FAEA-4E37-BA66-38391A10E556}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.19921875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.09765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.69921875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="32.8984375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="28.69921875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24.796875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="38.8984375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="9">
+        <v>20</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="9">
+        <v>22</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{A131941C-424D-47AC-8CEA-84C137E1C01E}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{B84F2145-D9AB-4E82-8F92-79930171B1A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02624BC6-C98F-441A-AFE3-9DF3E67DC643}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="32.59765625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="29.59765625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="43" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.796875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3:D6" r:id="rId1" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{D982E710-5C33-4493-8A4C-4A1E6D65FAAA}"/>
+    <hyperlink ref="E3:E6" r:id="rId2" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{B91985A6-2B86-426A-8A8E-176B9629E0B9}"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{7EEBE83E-9409-4B9A-8E88-38F223C22D5D}"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{BA3B3055-B57B-4BB1-9E81-FE9C5F20339B}"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{06843540-37A2-474E-B43D-62365296E5B7}"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{FCE9C49E-B105-41B6-B879-68A7805BA1C9}"/>
+    <hyperlink ref="E5" r:id="rId7" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{C98E2C10-B41F-4D72-A797-BAD956518008}"/>
+    <hyperlink ref="E6" r:id="rId8" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{FBAAD513-E2AC-4E36-B629-5CA38ACC869A}"/>
+    <hyperlink ref="E7" r:id="rId9" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{7077C090-D4F2-4638-83FB-33E1456D56BA}"/>
+    <hyperlink ref="E8" r:id="rId10" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{CD2F84CC-DEFD-4F62-BC04-99A47B92E177}"/>
+    <hyperlink ref="D2:D3" r:id="rId11" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{B2A42ADE-80D8-4302-B806-E4B141F0E16C}"/>
+    <hyperlink ref="E2:E3" r:id="rId12" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{529CE9BF-7890-45C3-A423-E0B08DDBB87C}"/>
+    <hyperlink ref="D3" r:id="rId13" display="https://demo.activeitzone.com/ecommerce/login" xr:uid="{414BA5F5-E760-4AF3-A166-5BEB9CB03F31}"/>
+    <hyperlink ref="E3" r:id="rId14" display="https://demo.activeitzone.com/ecommerce/admin" xr:uid="{9E467EF7-81D2-4E0C-BD80-262848D9184B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435FD99C-E142-4108-9047-23A4C7FFA60C}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.19921875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.09765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.69921875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="32.8984375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="28.69921875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24.796875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="38.8984375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="9">
+        <v>20</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="9">
+        <v>22</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{15DA40C9-5E4C-4651-B108-C8736DB8DF92}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{D15723D7-790B-45D4-B411-9628D1DE8F80}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{7E3F0BC7-F319-4F74-A3B2-647B6AE17606}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>